<commit_message>
improve GetCellFormat and GetCellValue
</commit_message>
<xml_diff>
--- a/Excelam.Tests/Files/Cells/GetManyCellFormatValues.xlsx
+++ b/Excelam.Tests/Files/Cells/GetManyCellFormatValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/70-yvlawy/Excelam/Dev/ExcelamSol/Excelam.Tests/Files/Cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3FEF3E4-552D-43F0-B0CF-1268EE8B692F}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9A29895-E467-417E-B860-6A5EBA4544A5}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="18945" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>bonjour</t>
   </si>
@@ -94,9 +94,6 @@
     <t>heure</t>
   </si>
   <si>
-    <t>compta</t>
-  </si>
-  <si>
     <t>monétaire</t>
   </si>
   <si>
@@ -104,13 +101,25 @@
   </si>
   <si>
     <t>a formula</t>
+  </si>
+  <si>
+    <t>compta €</t>
+  </si>
+  <si>
+    <t>accounting € euro</t>
+  </si>
+  <si>
+    <t>accounting € Anglais Irlande</t>
+  </si>
+  <si>
+    <t>accounting $ anglais - canada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="11">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
@@ -118,7 +127,10 @@
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="171" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -176,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -196,7 +208,10 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,15 +492,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
@@ -493,7 +508,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,7 +573,7 @@
         <v>4.5599999999999998E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <f>SUM(E5:E6)</f>
@@ -631,7 +646,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" s="17">
         <v>45.21</v>
@@ -639,7 +654,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="18">
         <v>88.22</v>
@@ -647,10 +662,34 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="19">
         <v>91.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="20">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="21">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="22">
+        <v>4.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>